<commit_message>
Highlight the columns needed
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naren/Documents/GIT/LendingClubCaseStudy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rabia/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EE8F1B-51A4-FD43-82F7-83ED8D948344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FA7164C-AA71-7F42-A401-45F496C17B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
     <sheet name="RejectStats" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$116</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
@@ -942,7 +942,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1125,6 +1125,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1363,7 +1375,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1406,6 +1418,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1501,7 +1518,31 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1527,8 +1568,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1829,14 +1870,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A103" sqref="A103:A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1855,8 +1896,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>229</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1864,8 +1905,8 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>233</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1873,8 +1914,8 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1882,8 +1923,8 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:4" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>223</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1891,8 +1932,8 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1900,8 +1941,8 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
         <v>191</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1909,8 +1950,8 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
         <v>189</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1918,8 +1959,8 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>108</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1927,8 +1968,8 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>234</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1936,8 +1977,8 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>235</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1945,8 +1986,8 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>99</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1954,8 +1995,8 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
         <v>165</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1963,8 +2004,8 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
         <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1972,8 +2013,8 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1981,8 +2022,8 @@
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>236</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1990,863 +2031,863 @@
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>55</v>
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>179</v>
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>193</v>
+    <row r="19" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>23</v>
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>186</v>
+        <v>56</v>
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>10</v>
+    <row r="21" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>197</v>
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>154</v>
+    <row r="22" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>197</v>
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>24</v>
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>3</v>
+    <row r="25" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>160</v>
+    <row r="26" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
+    <row r="27" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>58</v>
+    <row r="28" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
+    <row r="29" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="C29" s="20"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>216</v>
+    <row r="30" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="C30" s="20"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>34</v>
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="30" t="s">
+        <v>7</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>226</v>
+    <row r="32" spans="1:3" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>228</v>
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>199</v>
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>61</v>
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>82</v>
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>13</v>
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="30" t="s">
+        <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5"/>
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>45</v>
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="30" t="s">
+        <v>14</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>200</v>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>222</v>
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>201</v>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>92</v>
+    <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>187</v>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>62</v>
+    <row r="43" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>83</v>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>222</v>
+    <row r="45" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>63</v>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="D46" s="4"/>
       <c r="I46" s="10"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>126</v>
+    <row r="47" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D47" s="4"/>
       <c r="I47" s="10"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>127</v>
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="D48" s="4"/>
       <c r="I48" s="12"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
-        <v>119</v>
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="29" t="s">
+        <v>239</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
-        <v>105</v>
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="29" t="s">
+        <v>240</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>129</v>
+        <v>241</v>
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>238</v>
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="29" t="s">
+        <v>242</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>65</v>
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>130</v>
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>66</v>
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>212</v>
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>239</v>
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="26" t="s">
+        <v>111</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>240</v>
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="26" t="s">
+        <v>109</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>241</v>
+        <v>135</v>
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
-        <v>242</v>
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
-        <v>243</v>
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="26" t="s">
+        <v>121</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>93</v>
+    <row r="60" spans="1:4" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="9" t="s">
-        <v>98</v>
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="26" t="s">
+        <v>120</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="9" t="s">
-        <v>110</v>
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="26" t="s">
+        <v>103</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
-        <v>117</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="26" t="s">
+        <v>115</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
-        <v>111</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="26" t="s">
+        <v>114</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
-        <v>109</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="26" t="s">
+        <v>113</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="9" t="s">
-        <v>116</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="26" t="s">
+        <v>104</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>220</v>
       </c>
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>29</v>
+    <row r="74" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>35</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>36</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
-        <v>97</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>18</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
-        <v>107</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="26" t="s">
+        <v>158</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B105" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>88</v>
+        <v>45</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>90</v>
+        <v>1</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" s="24" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C113" s="23"/>
+    </row>
+    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B113" s="22" t="s">
+      <c r="B116" s="22" t="s">
         <v>81</v>
-      </c>
-      <c r="C113" s="23"/>
-    </row>
-    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B115" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="B116" s="16" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -2855,9 +2896,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B57" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:B116" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B116">
-      <sortCondition ref="A1:A116"/>
+      <sortCondition sortBy="cellColor" ref="A1:A116" dxfId="2"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">

</xml_diff>